<commit_message>
Update default indicator sample excel
</commit_message>
<xml_diff>
--- a/public/excel-templates/GBF-INDICATORS-DATA.xlsx
+++ b/public/excel-templates/GBF-INDICATORS-DATA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blaisefonseca/Projects/online-reporting-tool/public/excel-templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D54DAA26-BD2A-4448-8CDF-13D9BB475791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591BE202-52CE-134A-9E81-B11A93579382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4080" yWindow="500" windowWidth="30240" windowHeight="17740" xr2:uid="{BF91B3EE-77EB-4227-9B95-5DA7E436E5B2}"/>
   </bookViews>
@@ -35,24 +35,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={C67889F9-8025-41A8-B7D9-325B23FD2960}</author>
-  </authors>
-  <commentList>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{C67889F9-8025-41A8-B7D9-325B23FD2960}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Add rows for each year. </t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
@@ -109,10 +91,10 @@
     <t>Benefits received by indigenous peoples and local communities</t>
   </si>
   <si>
-    <t>Indicator_code</t>
-  </si>
-  <si>
     <t>C.1</t>
+  </si>
+  <si>
+    <t>Indicator code</t>
   </si>
 </sst>
 </file>
@@ -189,9 +171,7 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Jillian Campbell" id="{D519B181-81A4-4322-8EC7-262A77C1FCD8}" userId="S::campbell7@un.org::3a9f94b7-d4a3-460f-b437-2d7c8a57bdc0" providerId="AD"/>
-</personList>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -509,20 +489,12 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="E1" dT="2024-04-30T19:46:21.41" personId="{D519B181-81A4-4322-8EC7-262A77C1FCD8}" id="{C67889F9-8025-41A8-B7D9-325B23FD2960}">
-    <text xml:space="preserve">Add rows for each year. </text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66986885-9186-4720-8DB3-794DF0DD364C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66986885-9186-4720-8DB3-794DF0DD364C}">
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -540,7 +512,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -566,7 +538,7 @@
     </row>
     <row r="2" spans="1:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>13</v>
@@ -592,7 +564,7 @@
     </row>
     <row r="3" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>14</v>
@@ -619,6 +591,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>